<commit_message>
- Added all Buildings to InfluenceData - Added new Documents to folder
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -144,9 +144,6 @@
     <t>Observatory</t>
   </si>
   <si>
-    <t>Botanical Garden (Glasshouse</t>
-  </si>
-  <si>
     <t>Church</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>Vegetables and fruit storage</t>
+  </si>
+  <si>
+    <t>Botanical Garden (Glasshouse)</t>
   </si>
 </sst>
 </file>
@@ -486,12 +486,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -501,18 +495,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -540,331 +533,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1350,7 +1018,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1030,7 @@
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="17"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
@@ -1383,15 +1051,15 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="22" t="s">
+      <c r="F1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1409,14 +1077,14 @@
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="12"/>
-      <c r="H2" s="23">
+      <c r="H2" s="21">
         <v>5</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1434,14 +1102,14 @@
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="12"/>
-      <c r="H3" s="24">
+      <c r="H3" s="22">
         <v>1</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1459,16 +1127,16 @@
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="24">
+        <v>55</v>
+      </c>
+      <c r="H4" s="22">
         <v>3</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1486,14 +1154,14 @@
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="12"/>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <v>5</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1511,14 +1179,14 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="12"/>
-      <c r="H6" s="23">
+      <c r="H6" s="21">
         <v>5</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1536,14 +1204,14 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <v>4</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1561,14 +1229,14 @@
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="23">
+      <c r="H8" s="21">
         <v>3</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1586,14 +1254,14 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="12"/>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1601,7 +1269,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>9</v>
@@ -1611,14 +1279,14 @@
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="12"/>
-      <c r="H10" s="23">
+      <c r="H10" s="21">
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1626,7 +1294,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -1636,14 +1304,14 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="23">
+      <c r="H11" s="21">
         <v>3</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1661,14 +1329,14 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <v>3</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1686,14 +1354,14 @@
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="23">
+      <c r="H13" s="21">
         <v>3</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1711,14 +1379,14 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="H14" s="23">
+      <c r="H14" s="21">
         <v>3</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1736,14 +1404,14 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <v>3</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1761,14 +1429,14 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <v>2</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1786,14 +1454,14 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="24">
+      <c r="H17" s="22">
         <v>2</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1811,14 +1479,14 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="24">
+      <c r="H18" s="22">
         <v>4</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1836,14 +1504,14 @@
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="24">
+      <c r="H19" s="22">
         <v>5</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1861,14 +1529,14 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="H20" s="24">
+      <c r="H20" s="22">
         <v>3</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1886,14 +1554,14 @@
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="23">
+      <c r="H21" s="21">
         <v>4</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1911,14 +1579,14 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="H22" s="23">
+      <c r="H22" s="21">
         <v>2</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1936,14 +1604,14 @@
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="H23" s="23">
+      <c r="H23" s="21">
         <v>3</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1951,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>11</v>
@@ -1961,22 +1629,22 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="H24" s="23">
+      <c r="H24" s="21">
         <v>2</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>82</v>
+      <c r="B25" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>11</v>
@@ -1986,14 +1654,14 @@
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="H25" s="23">
+      <c r="H25" s="21">
         <v>5</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2011,14 +1679,14 @@
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="12"/>
-      <c r="H26" s="23">
+      <c r="H26" s="21">
         <v>3</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2036,14 +1704,14 @@
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="23">
+      <c r="H27" s="21">
         <v>5</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2061,14 +1729,14 @@
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="12"/>
-      <c r="H28" s="23">
+      <c r="H28" s="21">
         <v>3</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2076,7 +1744,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>12</v>
@@ -2086,14 +1754,14 @@
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G29" s="12"/>
-      <c r="H29" s="23">
+      <c r="H29" s="21">
         <v>3</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2101,7 +1769,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>13</v>
@@ -2111,14 +1779,14 @@
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="12"/>
-      <c r="H30" s="23">
+      <c r="H30" s="21">
         <v>5</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2126,7 +1794,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -2136,14 +1804,14 @@
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G31" s="12"/>
-      <c r="H31" s="23">
+      <c r="H31" s="21">
         <v>2</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2151,7 +1819,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>14</v>
@@ -2161,14 +1829,14 @@
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="12"/>
-      <c r="H32" s="23">
+      <c r="H32" s="21">
         <v>3</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2176,7 +1844,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>14</v>
@@ -2186,14 +1854,14 @@
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="23">
+      <c r="H33" s="21">
         <v>3</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2201,7 +1869,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>14</v>
@@ -2211,69 +1879,69 @@
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="12"/>
-      <c r="H34" s="23">
+      <c r="H34" s="21">
         <v>4</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="21" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2281,76 +1949,76 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H34">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2360,13 +2028,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Tetris">
+      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
+      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Block">
+      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2442,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2453,10 +2132,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,13 +2143,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,13 +2157,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2492,13 +2171,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,13 +2185,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2560,16 +2239,16 @@
         <v>21</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2580,16 +2259,16 @@
         <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2600,13 +2279,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2617,10 +2296,10 @@
         <v>26</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2631,7 +2310,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Added End of Level-flowchart - Updated Building List
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nold Slaine\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CA065E-EF4A-43C3-BEFB-CED58D5A6404}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="21315" windowHeight="10050"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Building-List" sheetId="1" r:id="rId1"/>
     <sheet name="Island" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
+    <sheet name="Building-List NEW" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -265,12 +272,24 @@
   </si>
   <si>
     <t>Botanical Garden (Glasshouse)</t>
+  </si>
+  <si>
+    <t>Inselteile</t>
+  </si>
+  <si>
+    <t>Luftschiffe</t>
+  </si>
+  <si>
+    <t>Insel-Schmuck</t>
+  </si>
+  <si>
+    <t>Start-Gebäude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
@@ -505,7 +524,27 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -517,6 +556,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -533,6 +589,180 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -723,14 +953,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -768,9 +1001,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -803,9 +1036,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -838,9 +1088,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1013,12 +1280,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="A1:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1949,71 +2216,71 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2038,14 +2305,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
+      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
+      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
-      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Block">
-      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2053,25 +2320,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Lists!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576 G2:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Lists!$F$2:$F$4</xm:f>
           </x14:formula1>
@@ -2084,7 +2351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2199,7 +2466,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -2212,7 +2479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2339,4 +2606,866 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FBC69E-C915-42FD-99B8-4DD6DF451F73}">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="17"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="21">
+        <v>5</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="22">
+        <v>1</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="22">
+        <v>3</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="21">
+        <v>5</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="21">
+        <v>5</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="21">
+        <v>4</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="21">
+        <v>3</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="21">
+        <v>5</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="21">
+        <v>3</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="21">
+        <v>3</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="21">
+        <v>3</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="21">
+        <v>3</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="21">
+        <v>3</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="21">
+        <v>2</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="22">
+        <v>2</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="21">
+        <v>4</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="21">
+        <v>3</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="21">
+        <v>2</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>19</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="21">
+        <v>5</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="21">
+        <v>3</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="21">
+        <v>5</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="21">
+        <v>2</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="21">
+        <v>3</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="21">
+        <v>3</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="21">
+        <v>4</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C35:C1048576 C1:C26">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
+      <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
+      <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
+      <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
+      <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
+      <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
+      <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
+      <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
+      <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D1048576 D1:D26">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
+      <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
+      <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
+      <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
+      <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35:G1048576 F1:G26">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
+      <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
+      <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
+      <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
+      <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
+      <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
+      <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35:I1048576 I1:I26">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
+      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
+      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
+      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:H1048576 H1:H26">
+    <cfRule type="colorScale" priority="317">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H26">
+    <cfRule type="colorScale" priority="321">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8AE22987-91BE-4CC1-A83C-E1B46CA4795E}">
+          <x14:formula1>
+            <xm:f>Lists!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I35:I1048576 I2:I26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C78FFF5C-9BB9-49AB-9E74-8A1B5D54F03F}">
+          <x14:formula1>
+            <xm:f>Lists!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F35:G1048576 F2:G26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{05D1FD66-FCEC-469B-B470-D7AB103F4A0A}">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D35:D1048576 D1:D26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{71FE88DB-20AC-42D8-8FF1-051CFF80989E}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C35:C1048576 C2:C26</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated Buliding List - Added new Matrix
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nold Slaine\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CA065E-EF4A-43C3-BEFB-CED58D5A6404}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Building-List" sheetId="1" r:id="rId1"/>
+    <sheet name="Building-List" sheetId="4" r:id="rId1"/>
     <sheet name="Island" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
-    <sheet name="Building-List NEW" sheetId="4" r:id="rId4"/>
+    <sheet name="Building-List OLD" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -289,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
@@ -961,9 +955,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1001,9 +995,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1036,26 +1030,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1088,26 +1065,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1280,12 +1240,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="A1:I34"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1439,10 +1399,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11" t="s">
@@ -1464,7 +1424,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>26</v>
@@ -1489,7 +1449,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>26</v>
@@ -1514,7 +1474,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>22</v>
@@ -1536,13 +1496,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
@@ -1550,7 +1510,7 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>69</v>
@@ -1561,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -1578,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1586,7 +1546,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>10</v>
@@ -1596,7 +1556,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="21">
@@ -1611,17 +1571,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="21">
@@ -1636,7 +1596,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>10</v>
@@ -1661,7 +1621,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
@@ -1675,10 +1635,10 @@
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1686,24 +1646,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" s="21">
+      <c r="H16" s="22">
         <v>2</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>69</v>
+      <c r="I16" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1711,24 +1671,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="22">
-        <v>2</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>60</v>
+      <c r="H17" s="21">
+        <v>4</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1736,24 +1696,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="22">
-        <v>4</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>69</v>
+      <c r="H18" s="21">
+        <v>3</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1761,49 +1721,49 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="22">
-        <v>5</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>69</v>
+      <c r="H19" s="21">
+        <v>2</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>35</v>
+      <c r="B20" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="H20" s="22">
-        <v>3</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>60</v>
+      <c r="H20" s="21">
+        <v>5</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1811,13 +1771,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
@@ -1825,7 +1785,7 @@
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>68</v>
@@ -1836,10 +1796,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>23</v>
@@ -1850,10 +1810,10 @@
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1861,24 +1821,24 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1886,21 +1846,21 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>68</v>
@@ -1910,11 +1870,11 @@
       <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>81</v>
+      <c r="B25" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>26</v>
@@ -1925,7 +1885,7 @@
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>68</v>
@@ -1936,13 +1896,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
@@ -1950,342 +1910,144 @@
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <v>26</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="21">
-        <v>5</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
+    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>27</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="21">
-        <v>3</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>69</v>
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>28</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="21">
-        <v>3</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>68</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>29</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="21">
-        <v>5</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>30</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="21">
-        <v>2</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>69</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>31</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="21">
-        <v>3</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>32</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="21">
-        <v>3</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="21">
-        <v>4</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="19" t="s">
-        <v>79</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
+  <conditionalFormatting sqref="C35:C1048576 C1:C26">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
+  <conditionalFormatting sqref="D35:D1048576 D1:D26">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
+  <conditionalFormatting sqref="F35:G1048576 F1:G26">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="I35:I1048576 I1:I26">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
+      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
+      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
+      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:H1048576 H1:H26">
+    <cfRule type="colorScale" priority="317">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2294,8 +2056,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="H2:H26">
+    <cfRule type="colorScale" priority="321">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2304,45 +2066,34 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
-      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
-      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
-      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I35:I1048576 I2:I26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F35:G1048576 F2:G26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D35:D1048576 D1:D26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>Lists!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>Lists!$D$2:$D$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576 G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>Lists!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>C35:C1048576 C2:C26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2351,7 +2102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2466,7 +2217,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -2479,7 +2230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2609,12 +2360,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FBC69E-C915-42FD-99B8-4DD6DF451F73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2519,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>26</v>
@@ -2793,7 +2544,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>26</v>
@@ -2818,7 +2569,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>26</v>
@@ -2843,7 +2594,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>22</v>
@@ -2865,13 +2616,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
@@ -2879,7 +2630,7 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>69</v>
@@ -2890,7 +2641,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -2900,14 +2651,14 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="21">
         <v>3</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2915,7 +2666,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>10</v>
@@ -2940,17 +2691,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="21">
@@ -2965,7 +2716,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>10</v>
@@ -2990,7 +2741,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
@@ -3004,10 +2755,10 @@
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3015,24 +2766,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <v>2</v>
       </c>
-      <c r="I16" s="18" t="s">
-        <v>60</v>
+      <c r="I16" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3040,24 +2791,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="21">
-        <v>4</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>68</v>
+      <c r="H17" s="22">
+        <v>2</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3065,24 +2816,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="H18" s="21">
-        <v>3</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>68</v>
+      <c r="H18" s="22">
+        <v>4</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3090,49 +2841,49 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" s="21">
-        <v>2</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>68</v>
+      <c r="H19" s="22">
+        <v>5</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>81</v>
+      <c r="B20" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="H20" s="21">
-        <v>5</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>68</v>
+      <c r="H20" s="22">
+        <v>3</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3140,13 +2891,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
@@ -3154,7 +2905,7 @@
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>68</v>
@@ -3165,10 +2916,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>23</v>
@@ -3179,10 +2930,10 @@
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3190,24 +2941,24 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3215,21 +2966,21 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>68</v>
@@ -3239,11 +2990,11 @@
       <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>45</v>
+      <c r="B25" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>26</v>
@@ -3254,7 +3005,7 @@
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>68</v>
@@ -3265,13 +3016,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
@@ -3279,144 +3030,342 @@
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="21">
+        <v>5</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="21">
+        <v>3</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>83</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="21">
+        <v>3</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>28</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="21">
+        <v>5</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>85</v>
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="21">
+        <v>2</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>30</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="21">
+        <v>3</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="21">
+        <v>3</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="21">
+        <v>4</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C35:C1048576 C1:C26">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D1048576 D1:D26">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35:G1048576 F1:G26">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:I1048576 I1:I26">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
-      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
-      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
-      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35:H1048576 H1:H26">
-    <cfRule type="colorScale" priority="317">
+  <conditionalFormatting sqref="H2:H34">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3425,8 +3374,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
-    <cfRule type="colorScale" priority="321">
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3435,34 +3384,45 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
+      <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
+      <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
+      <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8AE22987-91BE-4CC1-A83C-E1B46CA4795E}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576 G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I35:I1048576 I2:I26</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C78FFF5C-9BB9-49AB-9E74-8A1B5D54F03F}">
-          <x14:formula1>
-            <xm:f>Lists!$D$2:$D$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F35:G1048576 F2:G26</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{05D1FD66-FCEC-469B-B470-D7AB103F4A0A}">
-          <x14:formula1>
-            <xm:f>Lists!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D35:D1048576 D1:D26</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{71FE88DB-20AC-42D8-8FF1-051CFF80989E}">
-          <x14:formula1>
-            <xm:f>Lists!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>C35:C1048576 C2:C26</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
. Added Island Concept - Added new shapes - updated Buliding list & Matrix
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Building-List" sheetId="4" r:id="rId1"/>
@@ -1243,9 +1243,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1967,82 +1967,82 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C35:C1048576 C1:C26">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D1048576 D1:D26">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:G1048576 F1:G26">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:I1048576 I1:I26">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2363,7 +2363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
@@ -3296,71 +3296,71 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3385,13 +3385,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- Updated Building List - Updated Helios Matrix - Ignored tmp folder for google drive
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -278,6 +278,24 @@
   </si>
   <si>
     <t>Start-Gebäude</t>
+  </si>
+  <si>
+    <t>Circus</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Fountain</t>
+  </si>
+  <si>
+    <t>Resource Docks</t>
+  </si>
+  <si>
+    <t>Start Building</t>
   </si>
 </sst>
 </file>
@@ -518,7 +536,218 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1245,7 +1474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1625,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
@@ -1521,7 +1750,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -1546,13 +1775,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
@@ -1571,7 +1800,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
@@ -1596,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>10</v>
@@ -1610,10 +1839,10 @@
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1621,24 +1850,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="H15" s="21">
+      <c r="H15" s="22">
         <v>2</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>69</v>
+      <c r="I15" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1646,24 +1875,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" s="22">
-        <v>2</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>60</v>
+      <c r="H16" s="21">
+        <v>4</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1671,21 +1900,21 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>68</v>
@@ -1696,7 +1925,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>11</v>
@@ -1710,7 +1939,7 @@
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>68</v>
@@ -1720,22 +1949,22 @@
       <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>80</v>
+      <c r="B19" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>68</v>
@@ -1745,14 +1974,14 @@
       <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>81</v>
+      <c r="B20" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
@@ -1760,7 +1989,7 @@
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>68</v>
@@ -1771,13 +2000,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
@@ -1785,10 +2014,10 @@
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1796,7 +2025,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>14</v>
@@ -1810,7 +2039,7 @@
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>69</v>
@@ -1821,13 +2050,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
@@ -1835,10 +2064,10 @@
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1846,13 +2075,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
@@ -1871,13 +2100,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="11" t="s">
@@ -1885,7 +2114,7 @@
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>68</v>
@@ -1896,10 +2125,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>23</v>
@@ -1910,7 +2139,7 @@
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>68</v>
@@ -1919,7 +2148,7 @@
     <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>48</v>
@@ -1927,7 +2156,7 @@
     </row>
     <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>83</v>
@@ -1935,7 +2164,7 @@
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>84</v>
@@ -1943,7 +2172,7 @@
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>85</v>
@@ -1951,7 +2180,7 @@
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>86</v>
@@ -1967,82 +2196,82 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C35:C1048576 C1:C26">
-    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="71" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="70" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="69" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="68" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="67" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="66" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="65" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="64" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D1048576 D1:D26">
-    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="58" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:G1048576 F1:G26">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="52" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="51" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:I1048576 I1:I26">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3296,71 +3525,71 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3385,13 +3614,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- Updated GD Data
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -536,218 +536,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1472,9 +1261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2139,7 +1928,7 @@
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>68</v>
@@ -2196,82 +1985,82 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C35:C1048576 C1:C26">
-    <cfRule type="containsText" dxfId="71" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D1048576 D1:D26">
-    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:G1048576 F1:G26">
-    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:I1048576 I1:I26">
-    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3525,71 +3314,71 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Decorations">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Decorations">
       <formula>NOT(ISERROR(SEARCH("Decorations",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Spirituality">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Spirituality">
       <formula>NOT(ISERROR(SEARCH("Spirituality",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Culture">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Culture">
       <formula>NOT(ISERROR(SEARCH("Culture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Agriculture">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Agriculture">
       <formula>NOT(ISERROR(SEARCH("Agriculture",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Industry">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Industry">
       <formula>NOT(ISERROR(SEARCH("Industry",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Services">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="Services">
       <formula>NOT(ISERROR(SEARCH("Services",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="City">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="City">
       <formula>NOT(ISERROR(SEARCH("City",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Exclusive">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="Exclusive">
       <formula>NOT(ISERROR(SEARCH("Exclusive",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Noble">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Noble">
       <formula>NOT(ISERROR(SEARCH("Noble",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="Sand">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Sand">
       <formula>NOT(ISERROR(SEARCH("Sand",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="Cliff">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cliff">
       <formula>NOT(ISERROR(SEARCH("Cliff",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Grass">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Grass">
       <formula>NOT(ISERROR(SEARCH("Grass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Rock">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Rock">
       <formula>NOT(ISERROR(SEARCH("Rock",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3614,13 +3403,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Block">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Block">
       <formula>NOT(ISERROR(SEARCH("Block",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Special">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Special">
       <formula>NOT(ISERROR(SEARCH("Special",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Tetris">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Tetris">
       <formula>NOT(ISERROR(SEARCH("Tetris",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- Updated Buildings to new List - Updated Documents - Changed Difficulty (Bit more challenging) - Updated Decks & Building Connections
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>Start Building</t>
+  </si>
+  <si>
+    <t>Power Distributor</t>
+  </si>
+  <si>
+    <t>Power Plant</t>
+  </si>
+  <si>
+    <t>Mine</t>
+  </si>
+  <si>
+    <t>Erz-Ansammlung</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1275,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1526,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>10</v>
@@ -1564,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>10</v>
@@ -1639,7 +1651,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
@@ -1948,7 +1960,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1956,7 +1968,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1964,7 +1976,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1972,12 +1984,19 @@
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>30</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Balance iteration 2 - Added second testmap
</commit_message>
<xml_diff>
--- a/Documents/Building_List.xlsx
+++ b/Documents/Building_List.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Building-List" sheetId="4" r:id="rId1"/>
     <sheet name="Island" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
     <sheet name="Building-List OLD" sheetId="1" r:id="rId4"/>
+    <sheet name="Deck-Names" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -308,6 +309,48 @@
   </si>
   <si>
     <t>Erz-Ansammlung</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Pleasure</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Metall</t>
+  </si>
+  <si>
+    <t>GettingDrunk</t>
+  </si>
+  <si>
+    <t>Storehouse</t>
+  </si>
+  <si>
+    <t>Outlook</t>
+  </si>
+  <si>
+    <t>Booze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belief </t>
+  </si>
+  <si>
+    <t>Artwork</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Knowledge</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
@@ -3465,4 +3508,142 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>